<commit_message>
pep 8 standard compliance done for now with an average pylint score of 9.51 score o
</commit_message>
<xml_diff>
--- a/BioSANS/src/pylint_summary.xlsx
+++ b/BioSANS/src/pylint_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efaji\Documents\GitHub\SysBioSoft\BioSANS\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002D9108-2E4E-4609-A681-9BF565A06A2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FA2FA7-96BF-447B-890E-58DB5018548D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{45186604-A599-44EF-A531-3523BADC311A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="50">
   <si>
     <t>BioSANS.py</t>
   </si>
@@ -163,13 +163,25 @@
   </si>
   <si>
     <t>analytical_sol.py</t>
+  </si>
+  <si>
+    <t>lna_approx2.py</t>
+  </si>
+  <si>
+    <t>Python Files</t>
+  </si>
+  <si>
+    <t>Pylint score</t>
+  </si>
+  <si>
+    <t>Table 1. Pylint scores of python files in BioSANS2020 package</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,8 +189,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,8 +216,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -200,13 +231,84 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89223720-363C-465D-9C2D-ACD6FA28563B}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="M37" sqref="M37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,594 +634,879 @@
     <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" s="1">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="F2" s="1">
+        <v>10</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="B3" s="1">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="F3" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1">
+        <v>10</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="9">
+        <v>10</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="9">
+        <v>9.5833333333333304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="B5" s="1">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="F5" s="1">
+        <v>10</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="11">
+        <v>10</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="11">
+        <v>9.5284872298624705</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="B6" s="1">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="F6" s="1">
+        <v>10</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="11">
+        <v>10</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="11">
+        <v>9.4174757281553401</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1">
-        <v>10</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="B7" s="1">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="F7" s="1">
+        <v>10</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="11">
+        <v>10</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="11">
+        <v>9.4174757281553401</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="1">
-        <v>10</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="B8" s="1">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="F8" s="1">
+        <v>10</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="11">
+        <v>10</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" s="11">
+        <v>9.4117647058823497</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="1">
-        <v>10</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="B9" s="1">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="F9" s="1">
+        <v>10</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="11">
+        <v>10</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="11">
+        <v>9.4039735099337705</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B10" s="1">
         <v>9.8689956331877706</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F10" s="1">
         <v>9.8689956331877706</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="I10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="11">
+        <v>10</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="11">
+        <v>9.3975903614457792</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B11" s="1">
         <v>9.8591549295774605</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F11" s="1">
         <v>9.8538011695906391</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="I11" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="11">
+        <v>10</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" s="11">
+        <v>9.375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B12" s="1">
         <v>9.8412698412698401</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F12" s="1">
         <v>9.8412698412698401</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="I12" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="J12" s="11">
+        <v>9.8689956331877706</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="11">
+        <v>9.3617021276595693</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B13" s="1">
         <v>9.8000000000000007</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F13" s="1">
         <v>9.8000000000000007</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="I13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="11">
+        <v>9.8538011695906391</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L13" s="11">
+        <v>9.3081761006289305</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B14" s="1">
         <v>9.7619047619047592</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F14" s="1">
         <v>9.7619047619047592</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="I14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="11">
+        <v>9.8412698412698401</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="L14" s="11">
+        <v>9.2807017543859605</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B15" s="1">
         <v>9.7305389221556808</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F15" s="1">
         <v>9.7305389221556808</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="I15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="11">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L15" s="11">
+        <v>9.2708333333333304</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B16" s="1">
         <v>9.7196261682242895</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F16" s="1">
         <v>9.7196261682242895</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="I16" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="11">
+        <v>9.7619047619047592</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="L16" s="11">
+        <v>9.24657534246575</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B17" s="1">
         <v>9.6938775510203996</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F17" s="1">
         <v>9.6938775510203996</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="I17" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="11">
+        <v>9.7305389221556808</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L17" s="11">
+        <v>9.1891891891891895</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B18" s="1">
         <v>9.6812749003983996</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F18" s="1">
         <v>9.6812749003983996</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="I18" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="11">
+        <v>9.7233201581027604</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="L18" s="11">
+        <v>9.1891891891891895</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B19" s="1">
         <v>9.6272727272727199</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F19" s="1">
         <v>9.6272727272727199</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="I19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" s="11">
+        <v>9.7196261682242895</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L19" s="11">
+        <v>9.0909090909090899</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B20" s="1">
         <v>9.5145631067961105</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F20" s="1">
         <v>9.6212121212121193</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="I20" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="11">
+        <v>9.6938775510203996</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="L20" s="11">
+        <v>9.03765690376569</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B21" s="1">
         <v>9.4174757281553401</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F21" s="1">
         <v>9.5833333333333304</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="I21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" s="11">
+        <v>9.6812749003983996</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="L21" s="11">
+        <v>8.9855072463768106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B22" s="1">
         <v>9.4117647058823497</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F22" s="1">
         <v>9.5284872298624705</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="I22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" s="11">
+        <v>9.6272727272727199</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L22" s="11">
+        <v>8.8695652173912993</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B23" s="1">
         <v>9.4039735099337705</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F23" s="1">
         <v>9.5145631067961105</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="I23" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J23" s="13">
+        <v>9.6212121212121193</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="L23" s="13">
+        <v>7.2727272727272698</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B24" s="1">
         <v>9.3975903614457792</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F24" s="1">
         <v>9.4174757281553401</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B25" s="1">
         <v>9.3582887700534698</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F25" s="1">
         <v>9.4117647058823497</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="I25" s="5"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="4"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B26" s="1">
         <v>9.3081761006289305</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F26" s="1">
         <v>9.4039735099337705</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B27" s="1">
         <v>9.2708333333333304</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F27" s="1">
         <v>9.3975903614457792</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B27" s="1">
-        <v>9.1891891891891895</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27" s="1">
-        <v>9.375</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="B28" s="1">
         <v>9.1891891891891895</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" s="1">
+        <v>9.375</v>
+      </c>
+      <c r="J28" s="3">
+        <f>AVERAGE(J4:J23,L4:L23)</f>
+        <v>9.5140231829782458</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="1">
+        <v>9.1891891891891895</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F29" s="1">
         <v>9.3150684931506795</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B30" s="1">
         <v>9.0434782608695592</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F30" s="1">
         <v>9.3081761006289305</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B31" s="1">
         <v>9.03765690376569</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F31" s="1">
         <v>9.2708333333333304</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>0</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>5.8407079646017701</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F31" s="1">
-        <v>9.1891891891891895</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32">
-        <v>5.7462686567164099</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="F32" s="1">
         <v>9.1891891891891895</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>5.7462686567164099</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F33" s="1">
+        <v>9.1891891891891895</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>34</v>
       </c>
-      <c r="B33">
+      <c r="B34">
         <v>5.0909090909090899</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F34" s="1">
         <v>9.1351351351351298</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>35</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <v>1.76991150442477</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F35" s="1">
         <v>9.0909090909090899</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>36</v>
       </c>
-      <c r="B35">
+      <c r="B36">
         <v>1.7482517482517399</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F36" s="1">
         <v>9.03765690376569</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>39</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <v>1.4776632302405499</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F37" s="1">
         <v>8.8695652173912993</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>2</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <v>1.4285714285714199</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E38" t="s">
         <v>0</v>
       </c>
-      <c r="F37">
+      <c r="F38">
         <v>5.8407079646017701</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>38</v>
       </c>
-      <c r="B38">
+      <c r="B39">
         <v>1.2781954887218001</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E39" t="s">
         <v>1</v>
       </c>
-      <c r="F38">
+      <c r="F39">
         <v>5.7462686567164099</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>37</v>
       </c>
-      <c r="B39">
+      <c r="B40">
         <v>-6.25</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E40" t="s">
         <v>2</v>
       </c>
-      <c r="F39">
+      <c r="F40">
         <v>5.71428571428571</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>40</v>
       </c>
-      <c r="B40">
+      <c r="B41">
         <v>-10.943025540275</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E41" t="s">
         <v>3</v>
       </c>
-      <c r="F40">
+      <c r="F41">
         <v>-20</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>3</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>-20</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E42" t="s">
         <v>41</v>
       </c>
-      <c r="F41">
+      <c r="F42">
         <v>-28.1422924901185</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>41</v>
       </c>
-      <c r="B42">
+      <c r="B43">
         <v>-28.1422924901185</v>
       </c>
     </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L46" s="3"/>
+    </row>
   </sheetData>
-  <sortState ref="E1:F41">
-    <sortCondition descending="1" ref="F1:F41"/>
+  <sortState ref="I2:J42">
+    <sortCondition descending="1" ref="J2:J42"/>
   </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="I2:L2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>